<commit_message>
Draft io and repo
</commit_message>
<xml_diff>
--- a/docs/Project_Info/Status Assumptions To Do.xlsx
+++ b/docs/Project_Info/Status Assumptions To Do.xlsx
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>To Do</t>
   </si>
@@ -98,6 +95,21 @@
   </si>
   <si>
     <t>Status (%)</t>
+  </si>
+  <si>
+    <t>1st April 2023</t>
+  </si>
+  <si>
+    <t>1st May 2023</t>
+  </si>
+  <si>
+    <t>1st July 2023</t>
+  </si>
+  <si>
+    <t>1st August 2023</t>
+  </si>
+  <si>
+    <t>30th September 2023</t>
   </si>
 </sst>
 </file>
@@ -138,9 +150,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -149,6 +158,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,80 +445,80 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="62.921875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.3828125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="7.07421875" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.23046875" style="3"/>
+    <col min="1" max="1" width="62.921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.4609375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.07421875" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
-        <v>45017</v>
-      </c>
-      <c r="C2" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>45047</v>
-      </c>
-      <c r="C3" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
-        <v>45108</v>
-      </c>
-      <c r="C4" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>45139</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4">
-        <v>45199</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4">
         <v>0</v>
       </c>
     </row>
@@ -520,60 +532,61 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="57.3828125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.23046875" style="1"/>
+    <col min="2" max="2" width="9.23046875" style="5"/>
+    <col min="3" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.5</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.5</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.4</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5">
         <v>0</v>
       </c>
     </row>
@@ -599,10 +612,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
@@ -610,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -618,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
@@ -626,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -634,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
@@ -642,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
@@ -650,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -658,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>